<commit_message>
traitement et nettoyage des données
</commit_message>
<xml_diff>
--- a/entrainementCSV/dataLess.xlsx
+++ b/entrainementCSV/dataLess.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t xml:space="preserve">Année 2021 - services de police</t>
   </si>
@@ -34,6 +34,12 @@
     <t xml:space="preserve">02</t>
   </si>
   <si>
+    <t xml:space="preserve">2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2B</t>
+  </si>
+  <si>
     <t xml:space="preserve">Périmètres</t>
   </si>
   <si>
@@ -44,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">DCCRS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCPJ</t>
   </si>
   <si>
     <t xml:space="preserve">Code index</t>
@@ -56,6 +65,7 @@
         <color rgb="FF0070C0"/>
         <rFont val="Palatino Linotype"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Libellé index</t>
     </r>
@@ -66,6 +76,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Palatino Linotype"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -75,6 +86,7 @@
         <sz val="12"/>
         <rFont val="Palatino Linotype"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">\ </t>
     </r>
@@ -85,6 +97,7 @@
         <color rgb="FFED7D31"/>
         <rFont val="Palatino Linotype"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CSP</t>
     </r>
@@ -112,6 +125,36 @@
   </si>
   <si>
     <t xml:space="preserve">CIAT DE CHATEAU THIERRY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMRA 2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPAFA AJACCIO CAMPO DELL ORO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPAFA BONIFACIO FIGARI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTPJ D'AJACCIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSP D'AJACCIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMRA 2B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPAFA BASTIA PORETTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPAFA CALVI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPAFT BASTIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSP DE BASTIA</t>
   </si>
   <si>
     <t xml:space="preserve">Règlements de compte entre malfaiteurs</t>
@@ -148,6 +191,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -168,12 +212,14 @@
       <sz val="12"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -181,6 +227,7 @@
       <color rgb="FF0070C0"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -188,6 +235,7 @@
       <color rgb="FF5B9BD5"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -195,24 +243,28 @@
       <color rgb="FFED7D31"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFED7D31"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0070C0"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -299,7 +351,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -312,11 +364,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -409,17 +473,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -451,292 +515,592 @@
       </c>
       <c r="J1" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>6</v>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="5" t="s">
+    <row r="3" customFormat="false" ht="49.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="F3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="G3" s="7" t="s">
         <v>17</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
+      <c r="A4" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="7" t="n">
+      <c r="B4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="O4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="n">
+      <c r="A5" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8" t="n">
+      <c r="B5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="n">
+      <c r="A6" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="7" t="n">
+      <c r="B6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="P6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="n">
+      <c r="A7" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="8" t="n">
+      <c r="B7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="n">
+      <c r="A8" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="7" t="n">
+      <c r="B8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="7" t="n">
+      <c r="G8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="10" t="n">
         <v>1</v>
+      </c>
+      <c r="K8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="O8" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="P8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" s="10" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="n">
+      <c r="A9" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="8" t="n">
+      <c r="B9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="n">
+      <c r="A10" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="7" t="n">
+      <c r="B10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10" t="n">
         <v>353</v>
       </c>
-      <c r="F10" s="7" t="n">
+      <c r="F10" s="10" t="n">
         <v>168</v>
       </c>
-      <c r="G10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="7" t="n">
+      <c r="G10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="10" t="n">
         <v>163</v>
+      </c>
+      <c r="K10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="O10" s="10" t="n">
+        <v>340</v>
+      </c>
+      <c r="P10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="R10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" s="10" t="n">
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>